<commit_message>
Preparacion de mapeo mediante excel
</commit_message>
<xml_diff>
--- a/db_data_extraction/InputPhotocalysisMapping.xlsx
+++ b/db_data_extraction/InputPhotocalysisMapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="145">
   <si>
     <t xml:space="preserve">Prefix</t>
   </si>
@@ -80,6 +80,24 @@
     <t xml:space="preserve">https://dbpedia.org/page/</t>
   </si>
   <si>
+    <t xml:space="preserve">qudt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://qudt.org/2.1/schema/qudt/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://qudt.org/vocab/unit/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chebi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -119,7 +137,7 @@
     <t xml:space="preserve">phcat:MaterialTransformationProcess</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.example.com/materialTransformastionProcess/{No_de_ref}</t>
+    <t xml:space="preserve">http://data.example.com/materialTransformastionProcess/{ID}</t>
   </si>
   <si>
     <t xml:space="preserve">Input</t>
@@ -128,13 +146,31 @@
     <t xml:space="preserve">phcat:Input</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.example.com/input/{No_de_ref}/</t>
+    <t xml:space="preserve">http://data.example.com/input/{ID}</t>
   </si>
   <si>
     <t xml:space="preserve">Condition</t>
   </si>
   <si>
     <t xml:space="preserve">phcat:Condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.example.com/condition/{ID}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.example.com/output/{ID}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:Eg</t>
   </si>
   <si>
     <r>
@@ -145,7 +181,193 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">http://data.example.com/condition/</t>
+      <t xml:space="preserve">http://data.example.com/eg/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{ID}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">BET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:BET</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://data.example.com/bet/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{ID}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chebi:CHEBI_24431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.example.com/chemical/{ID}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OutputCuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:OutputCuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.example.com/output_quantity/{ID}-{unit}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/journals.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/paper_references.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/authors.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/material_transformations.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/inputs.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/conditions.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/outputs.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/chemicals.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predicate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReferenceID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InnerRef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OuterRef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcterms:title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:doi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{DOI}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{title}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:abstract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Abstract}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Volume}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positiveInteger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Issue}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcterms:date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Year}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:pageStart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Pages}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dc:isPartOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{journalID}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ID}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">phcat:has</t>
     </r>
     <r>
       <rPr>
@@ -154,110 +376,17 @@
         <rFont val="Calibri"/>
         <family val="0"/>
       </rPr>
-      <t xml:space="preserve">{No_de_ref}/</t>
+      <t xml:space="preserve">MaterialTransformationProcess</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phcat:Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://data.example.com/output/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">journals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paper_references</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phcat_authors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">catalystsdata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Predicate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DataType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReferenceID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InnerRef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OuterRef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dcterms:title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{name}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bibo:doi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{DOI}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{title}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bibo:abstract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Abstract}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bibo:volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Volume}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">positiveInteger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bibo:issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Issue}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dcterms:date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Year}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bibo:pageStart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Pages}</t>
+    <t xml:space="preserve">{No_de_ref}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dc:creator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{paperID}</t>
   </si>
   <si>
     <t xml:space="preserve">schema:name</t>
@@ -273,6 +402,114 @@
   </si>
   <si>
     <t xml:space="preserve">schema:Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:reportedIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs:label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Catalyst_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:operationMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Operation_mode}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:hasReactionEg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:hasBET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:hasInput</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Material_transformation_id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:hasCondition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qudt:numericValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Eg_eV}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qudt:unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit:EV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qudt:Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{BET_m2_g}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit:M2-PER-GM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Chemical}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Percent}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:cristalStructure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{crystal_structure}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:hasChemical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:hasRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:{Role}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:MaterialTransformationRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:conditionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Type}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qudt:value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Quantity}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit:{Unit}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:hasOutputCuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:numericValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit:{QUDT_unit}</t>
   </si>
   <si>
     <t xml:space="preserve">FunctionID</t>
@@ -285,7 +522,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -341,7 +578,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -350,6 +587,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -402,7 +645,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -427,6 +670,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -443,6 +690,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,6 +703,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,11 +789,11 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.67"/>
@@ -643,11 +898,29 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1663,112 +1936,152 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="61.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="10.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="8.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="8"/>
+      <c r="A2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>45</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2760,10 +3073,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" display="http://data.example.com/author/{author_name}-{ID}"/>
-    <hyperlink ref="C5" r:id="rId2" display="http://data.example.com/materialTransformastionProcess/{No_de_ref}"/>
-    <hyperlink ref="C6" r:id="rId3" display="http://data.example.com/input/"/>
-    <hyperlink ref="C7" r:id="rId4" display="http://data.example.com/condition/"/>
-    <hyperlink ref="C8" r:id="rId5" display="http://data.example.com/output/"/>
+    <hyperlink ref="C6" r:id="rId2" display="http://data.example.com/input/"/>
+    <hyperlink ref="C7" r:id="rId3" display="http://data.example.com/condition/"/>
+    <hyperlink ref="C8" r:id="rId4" display="http://data.example.com/output/"/>
+    <hyperlink ref="C9" r:id="rId5" display="http://data.example.com/eg/"/>
+    <hyperlink ref="C10" r:id="rId6" display="http://data.example.com/bet/"/>
+    <hyperlink ref="C12" r:id="rId7" display="http://data.example.com/output_quantity/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2780,95 +3095,275 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:C1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="28.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="10.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="16.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="8" width="10.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="8" width="8.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="11.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="28.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="30.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="9" width="10.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="9" width="8.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="9" width="11.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3846,6 +4341,9 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3862,237 +4360,586 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:G1006"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="33.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="37.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="40.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="25.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="8" width="8.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="11.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="28.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="36.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="40.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="9" width="30.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="28.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="11.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="25.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="9" width="8.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="9" width="11.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>49</v>
+        <v>72</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F19" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="B26" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="0"/>
+      <c r="E29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="0"/>
+      <c r="E34" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="F35" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="B36" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="11"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="11"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="11"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B37" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5056,9 +5903,15 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://en.wikipedia.org/wiki/"/>
+    <hyperlink ref="C14" r:id="rId1" display="https://en.wikipedia.org/wiki/{country_name}"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5081,7 +5934,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.67"/>
@@ -5091,14 +5944,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>42</v>
+      <c r="A1" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>